<commit_message>
PM report to PMB
</commit_message>
<xml_diff>
--- a/Project-Management/PMB/Mantid Cross Facility Technique support.xlsx
+++ b/Project-Management/PMB/Mantid Cross Facility Technique support.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Powder Diffraction TOF" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Indirect Inelastic" sheetId="7" r:id="rId7"/>
     <sheet name="Muon" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1257,7 +1257,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmm\-yyyy"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1311,6 +1311,11 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1384,7 +1389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1508,10 +1513,25 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1797,11 +1817,11 @@
   </sheetPr>
   <dimension ref="A1:I1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1888,7 +1908,7 @@
       <c r="E5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="48" t="s">
         <v>22</v>
       </c>
       <c r="G5" s="17" t="s">
@@ -2056,11 +2076,11 @@
       <c r="B13" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
       <c r="F13" s="31"/>
       <c r="G13" s="8"/>
       <c r="H13" s="26"/>
@@ -11333,11 +11353,11 @@
   </sheetPr>
   <dimension ref="A1:G1013"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11519,7 +11539,7 @@
         <v>70</v>
       </c>
       <c r="D12" s="9"/>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="50" t="s">
         <v>71</v>
       </c>
       <c r="F12" s="23"/>
@@ -18633,10 +18653,10 @@
   <dimension ref="A1:G1039"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18809,7 +18829,7 @@
       <c r="D11" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="51" t="s">
         <v>78</v>
       </c>
       <c r="F11" s="26"/>
@@ -32483,7 +32503,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -32550,7 +32570,7 @@
       <c r="B5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="52" t="s">
         <v>160</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -32618,7 +32638,7 @@
       <c r="B9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="52" t="s">
         <v>166</v>
       </c>
       <c r="D9" s="19" t="s">
@@ -32687,14 +32707,14 @@
       <c r="B13" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="53" t="s">
         <v>180</v>
       </c>
       <c r="D13" s="42" t="s">
         <v>181</v>
       </c>
       <c r="E13" s="26"/>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="50" t="s">
         <v>185</v>
       </c>
       <c r="G13" s="4"/>
@@ -40019,10 +40039,10 @@
   <dimension ref="A1:G1031"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -47549,10 +47569,10 @@
   <dimension ref="A1:M1037"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -61466,7 +61486,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>